<commit_message>
Se arregla el flujo de archivos PREI y SAI
</commit_message>
<xml_diff>
--- a/Implementación/Facturas/xmls_extraidos.xlsx
+++ b/Implementación/Facturas/xmls_extraidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I181"/>
+  <dimension ref="A1:I197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8220,6 +8220,694 @@
         </is>
       </c>
     </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>1354D9E0-5D89-44D6-A4BB-E93417D95B5F</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>P-6585</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>2025-08-22T13:26:42</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>ADRIANA QUIROZ RODRIGUEZ</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>QURA720718KP7</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>010 000 0246 00 00 PROPOFOL. EMULSIÓN INYECTABLE.EMULSION INYECTABLE CADA AMPOLLETA O FRASCO AMPULA CONTIENE: EMULSION CON O SIN EDETATO DISODICO (DIHIDRATADO) 200 MG. ENVASE CON 5 AMPOLLETAS O FRASCOS AMPULA DE 20 ML.</t>
+        </is>
+      </c>
+      <c r="G182" t="n">
+        <v>250</v>
+      </c>
+      <c r="H182" t="n">
+        <v>23750</v>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>P-6585 ADRIANA QUIROZ RODRIGUEZ.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>F27BFC72-8E1B-404C-BAAF-D950102B1B09</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>P-6570</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>2025-08-22T11:15:31</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G183" t="n">
+        <v>1996</v>
+      </c>
+      <c r="H183" t="n">
+        <v>165668</v>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>P-6570 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>69D4D535-CF02-44A5-9A3D-2A632469B947</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>P-6571</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>2025-08-22T11:23:32</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G184" t="n">
+        <v>2146</v>
+      </c>
+      <c r="H184" t="n">
+        <v>178118</v>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>P-6571 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>9141F3EB-728B-47B4-BF84-FCEBBAC8BBE0</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>P-6572</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>2025-08-22T11:28:30</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G185" t="n">
+        <v>10</v>
+      </c>
+      <c r="H185" t="n">
+        <v>830</v>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>P-6572 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>43BC1517-6DA3-42FC-A35E-427E974F782B</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>P-6573</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>2025-08-22T11:34:32</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G186" t="n">
+        <v>83</v>
+      </c>
+      <c r="H186" t="n">
+        <v>6889</v>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>P-6573 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>0658F2A5-56B5-441C-B17B-D3246DF54929</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>P-6574</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>2025-08-22T11:45:14</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G187" t="n">
+        <v>25</v>
+      </c>
+      <c r="H187" t="n">
+        <v>2075</v>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>P-6574 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>C20465C7-5DAC-48D2-AC0F-EE780230D57A</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>P-6575</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>2025-08-22T11:51:56</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G188" t="n">
+        <v>4589</v>
+      </c>
+      <c r="H188" t="n">
+        <v>380887</v>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>P-6575 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>EE275B25-6ED4-4E22-86D5-FAB968BE5FDA</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>P-6576</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>2025-08-22T11:58:58</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G189" t="n">
+        <v>1124</v>
+      </c>
+      <c r="H189" t="n">
+        <v>93292</v>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>P-6576 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>870D6D18-E68B-4820-90D8-B10DCFF903A1</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>P-6577</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>2025-08-22T12:13:55</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G190" t="n">
+        <v>78</v>
+      </c>
+      <c r="H190" t="n">
+        <v>6474</v>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>P-6577 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>5E63D996-999D-46C3-AFD2-DDCE228778D9</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>P-6578</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>2025-08-22T12:22:18</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G191" t="n">
+        <v>1466</v>
+      </c>
+      <c r="H191" t="n">
+        <v>121678</v>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>P-6578 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>3159F584-4DF8-4738-AC55-E24CF40439E8</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>P-6579</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>2025-08-22T12:28:30</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G192" t="n">
+        <v>997</v>
+      </c>
+      <c r="H192" t="n">
+        <v>82751</v>
+      </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>P-6579 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>0F825E1A-03C5-40D7-80FD-938FC390CB0E</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>P-6580</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>2025-08-22T12:43:44</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G193" t="n">
+        <v>7300</v>
+      </c>
+      <c r="H193" t="n">
+        <v>605900</v>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>P-6580 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>5D8CB6F1-C222-46D1-84F8-2C2AF908F49B</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>P-6581</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>2025-08-22T12:48:23</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G194" t="n">
+        <v>7031</v>
+      </c>
+      <c r="H194" t="n">
+        <v>583573</v>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>P-6581 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>6D3D9676-C144-4E4E-A37C-F7E34ECAA50B</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>P-6582</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>2025-08-22T12:52:50</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G195" t="n">
+        <v>5067</v>
+      </c>
+      <c r="H195" t="n">
+        <v>420561</v>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>P-6582 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>4A28D11B-AD4A-401C-AE95-40A08BD9F166</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>P-6583</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>2025-08-22T12:57:42</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G196" t="n">
+        <v>1452</v>
+      </c>
+      <c r="H196" t="n">
+        <v>120516</v>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>P-6583 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>B0C51690-3829-4651-B664-769AB6FD94CC</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>P-6584</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>2025-08-22T13:01:11</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>INSTITUTO MEXICANO DEL SEGURO SOCIAL</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>IMS421231I45</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>010 000 4411 00 00 LATANOPROSTSOLUCION OFTALMICA CADA ML CONTIENE: LATANOPROST 50 MICROGRAMOS ENVASE CON UN FRASCO GOTERO CON 2.5 ML.</t>
+        </is>
+      </c>
+      <c r="G197" t="n">
+        <v>713</v>
+      </c>
+      <c r="H197" t="n">
+        <v>59179</v>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>P-6584 IMSS.xml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>